<commit_message>
Made joint dataset of Southbound and Northbound
also did a lil distribution analysis
</commit_message>
<xml_diff>
--- a/data analyses/weather, LoS, TimeofDay, DayofWeek keys.xlsx
+++ b/data analyses/weather, LoS, TimeofDay, DayofWeek keys.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Final year project - fyp - dissertation\simulation\data analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC1048A2C1D845DA5BDE58F0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{10FC70EC-97DC-416C-9A98-E3D3A1AFBD08}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC1048A2C1D845DA5BDE58F0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0669FE2-6346-4022-866F-52910DBCA54A}"/>
   <bookViews>
-    <workbookView xWindow="3430" yWindow="2160" windowWidth="14400" windowHeight="7360" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weather key" sheetId="1" r:id="rId1"/>
     <sheet name="level of service key" sheetId="2" r:id="rId2"/>
     <sheet name="Day of Week key" sheetId="3" r:id="rId3"/>
     <sheet name="Time of Day key" sheetId="4" r:id="rId4"/>
+    <sheet name="Description key" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Weather</t>
   </si>
@@ -184,6 +185,21 @@
   </si>
   <si>
     <t>21:00 to 23:59</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Northbound</t>
+  </si>
+  <si>
+    <t>Traffic toward Lagos Island</t>
+  </si>
+  <si>
+    <t>Southbound</t>
+  </si>
+  <si>
+    <t>Traffic to Berger, Ikeja (Mainland)</t>
   </si>
 </sst>
 </file>
@@ -856,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B085CE1-12E9-4285-BD2B-41AEE3D10E02}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -954,4 +970,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E95428-8691-4C77-AD9D-9EF5AA4BE21B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update on shiny r frontend
</commit_message>
<xml_diff>
--- a/data analyses/weather, LoS, TimeofDay, DayofWeek keys.xlsx
+++ b/data analyses/weather, LoS, TimeofDay, DayofWeek keys.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC1048A2C1D845DA5BDE58F0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0669FE2-6346-4022-866F-52910DBCA54A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="3440" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weather key" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -872,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B085CE1-12E9-4285-BD2B-41AEE3D10E02}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -976,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E95428-8691-4C77-AD9D-9EF5AA4BE21B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated r scripts to prevent overfitting. and improved ui of webapp
</commit_message>
<xml_diff>
--- a/data analyses/weather, LoS, TimeofDay, DayofWeek keys.xlsx
+++ b/data analyses/weather, LoS, TimeofDay, DayofWeek keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Final year project - fyp - dissertation\simulation\data analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92aeda1fcbb40775/Final year project - fyp - dissertation/simulation/data analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC1048A2C1D845DA5BDE58F0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0669FE2-6346-4022-866F-52910DBCA54A}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC1048A2C1D845DA5BDE58F0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{04F32237-B4FE-4457-B70B-6860A4CA76BC}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3440" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weather key" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -872,11 +872,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B085CE1-12E9-4285-BD2B-41AEE3D10E02}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -976,11 +979,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E95428-8691-4C77-AD9D-9EF5AA4BE21B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>